<commit_message>
adding names to beetles in BeetleBase.cs
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BeetleNameDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BeetleNameDefs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LD35\trunk\UnityProject\LD35\Assets\StaticDefinitions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="11520"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="38400" windowHeight="11520"/>
   </bookViews>
   <sheets>
     <sheet name="beetleNameDefs" sheetId="2" r:id="rId1"/>
@@ -1707,9 +1712,6 @@
     <t xml:space="preserve">Polyphylla decemlineata </t>
   </si>
   <si>
-    <t xml:space="preserve">Hippodamia tredecimpunctata tibialis </t>
-  </si>
-  <si>
     <t xml:space="preserve">Disonycha triangularis </t>
   </si>
   <si>
@@ -2286,9 +2288,6 @@
     <t xml:space="preserve">Xyleborus glabratus </t>
   </si>
   <si>
-    <t>Callidium antennatum hesperum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ips hunteri </t>
   </si>
   <si>
@@ -2814,9 +2813,6 @@
     <t xml:space="preserve">Cryptophagus varus </t>
   </si>
   <si>
-    <t xml:space="preserve">Diabrotica undecimpunctata undecimpunctata </t>
-  </si>
-  <si>
     <t xml:space="preserve">Agrilus sinuatus </t>
   </si>
   <si>
@@ -2895,9 +2891,6 @@
     <t xml:space="preserve">Chaetocnema denticulata </t>
   </si>
   <si>
-    <t xml:space="preserve">Coccinella transversoguttata richardsoni </t>
-  </si>
-  <si>
     <t xml:space="preserve">Gratiana boliviana </t>
   </si>
   <si>
@@ -3205,6 +3198,22 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diabrotica undecimpunctata
+undecimpunctata </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coccinella transversoguttata
+richardsoni </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hippodamia tredecimpunctata 
+tibialis </t>
+  </si>
+  <si>
+    <t>Callidium antennatum
+hesperum</t>
   </si>
 </sst>
 </file>
@@ -3246,9 +3255,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3521,7 +3533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3531,25 +3543,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C534"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3571,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3582,7 +3594,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3593,7 +3605,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3604,7 +3616,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -3615,7 +3627,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3626,7 +3638,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -3637,7 +3649,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3648,7 +3660,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3659,7 +3671,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3670,7 +3682,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3692,7 +3704,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3714,7 +3726,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3725,7 +3737,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3736,7 +3748,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3747,7 +3759,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3758,7 +3770,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3769,7 +3781,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3780,7 +3792,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3791,7 +3803,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3802,7 +3814,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -3813,7 +3825,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -3824,7 +3836,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3835,7 +3847,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3846,7 +3858,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3857,7 +3869,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3868,7 +3880,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3879,7 +3891,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3890,7 +3902,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3901,7 +3913,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3912,7 +3924,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3923,7 +3935,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3934,7 +3946,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3945,7 +3957,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,7 +3968,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3989,7 +4001,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -4000,7 +4012,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -4011,7 +4023,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -4044,7 +4056,7 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -4055,7 +4067,7 @@
         <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -4066,7 +4078,7 @@
         <v>47</v>
       </c>
       <c r="C48" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -4077,7 +4089,7 @@
         <v>48</v>
       </c>
       <c r="C49" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -4088,7 +4100,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4099,7 +4111,7 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>975</v>
+        <v>971</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4110,7 +4122,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>976</v>
+        <v>972</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4121,7 +4133,7 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -4143,18 +4155,18 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>55</v>
       </c>
-      <c r="C56" t="s">
-        <v>755</v>
+      <c r="C56" s="2" t="s">
+        <v>1061</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4165,7 +4177,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>978</v>
+        <v>974</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4176,7 +4188,7 @@
         <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -4187,7 +4199,7 @@
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -4198,7 +4210,7 @@
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -4209,7 +4221,7 @@
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -4220,7 +4232,7 @@
         <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -4231,7 +4243,7 @@
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4242,7 +4254,7 @@
         <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -4253,7 +4265,7 @@
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -4264,7 +4276,7 @@
         <v>65</v>
       </c>
       <c r="C66" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -4275,7 +4287,7 @@
         <v>66</v>
       </c>
       <c r="C67" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -4286,7 +4298,7 @@
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -4297,7 +4309,7 @@
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -4308,7 +4320,7 @@
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -4319,7 +4331,7 @@
         <v>70</v>
       </c>
       <c r="C71" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -4330,7 +4342,7 @@
         <v>71</v>
       </c>
       <c r="C72" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -4341,7 +4353,7 @@
         <v>72</v>
       </c>
       <c r="C73" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -4352,7 +4364,7 @@
         <v>73</v>
       </c>
       <c r="C74" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -4363,7 +4375,7 @@
         <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -4374,7 +4386,7 @@
         <v>75</v>
       </c>
       <c r="C76" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -4385,7 +4397,7 @@
         <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>979</v>
+        <v>975</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -4396,7 +4408,7 @@
         <v>77</v>
       </c>
       <c r="C78" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -4407,7 +4419,7 @@
         <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -4418,7 +4430,7 @@
         <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -4429,7 +4441,7 @@
         <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>980</v>
+        <v>976</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -4440,7 +4452,7 @@
         <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -4451,7 +4463,7 @@
         <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>981</v>
+        <v>977</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -4462,7 +4474,7 @@
         <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -4473,7 +4485,7 @@
         <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -4484,7 +4496,7 @@
         <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -4495,7 +4507,7 @@
         <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -4506,7 +4518,7 @@
         <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -4517,7 +4529,7 @@
         <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -4528,7 +4540,7 @@
         <v>89</v>
       </c>
       <c r="C90" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -4550,7 +4562,7 @@
         <v>91</v>
       </c>
       <c r="C92" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -4561,7 +4573,7 @@
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>982</v>
+        <v>978</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -4572,7 +4584,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -4583,7 +4595,7 @@
         <v>94</v>
       </c>
       <c r="C95" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -4594,7 +4606,7 @@
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>983</v>
+        <v>979</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -4605,7 +4617,7 @@
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -4616,7 +4628,7 @@
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -4627,7 +4639,7 @@
         <v>98</v>
       </c>
       <c r="C99" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -4638,7 +4650,7 @@
         <v>99</v>
       </c>
       <c r="C100" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -4649,7 +4661,7 @@
         <v>100</v>
       </c>
       <c r="C101" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -4660,7 +4672,7 @@
         <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>984</v>
+        <v>980</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -4671,7 +4683,7 @@
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>985</v>
+        <v>981</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -4682,7 +4694,7 @@
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -4693,7 +4705,7 @@
         <v>104</v>
       </c>
       <c r="C105" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -4704,7 +4716,7 @@
         <v>105</v>
       </c>
       <c r="C106" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -4726,7 +4738,7 @@
         <v>107</v>
       </c>
       <c r="C108" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -4737,7 +4749,7 @@
         <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>986</v>
+        <v>982</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4759,7 +4771,7 @@
         <v>110</v>
       </c>
       <c r="C111" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -4770,7 +4782,7 @@
         <v>111</v>
       </c>
       <c r="C112" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -4781,7 +4793,7 @@
         <v>112</v>
       </c>
       <c r="C113" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -4792,7 +4804,7 @@
         <v>113</v>
       </c>
       <c r="C114" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -4803,7 +4815,7 @@
         <v>114</v>
       </c>
       <c r="C115" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -4814,7 +4826,7 @@
         <v>115</v>
       </c>
       <c r="C116" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -4825,7 +4837,7 @@
         <v>116</v>
       </c>
       <c r="C117" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -4836,7 +4848,7 @@
         <v>117</v>
       </c>
       <c r="C118" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -4847,7 +4859,7 @@
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -4858,7 +4870,7 @@
         <v>119</v>
       </c>
       <c r="C120" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -4869,7 +4881,7 @@
         <v>120</v>
       </c>
       <c r="C121" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -4880,7 +4892,7 @@
         <v>121</v>
       </c>
       <c r="C122" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -4891,7 +4903,7 @@
         <v>122</v>
       </c>
       <c r="C123" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4902,7 +4914,7 @@
         <v>123</v>
       </c>
       <c r="C124" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4913,7 +4925,7 @@
         <v>124</v>
       </c>
       <c r="C125" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -4924,7 +4936,7 @@
         <v>125</v>
       </c>
       <c r="C126" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -4935,7 +4947,7 @@
         <v>126</v>
       </c>
       <c r="C127" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4946,7 +4958,7 @@
         <v>127</v>
       </c>
       <c r="C128" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4957,7 +4969,7 @@
         <v>128</v>
       </c>
       <c r="C129" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4968,7 +4980,7 @@
         <v>129</v>
       </c>
       <c r="C130" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -4979,7 +4991,7 @@
         <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -4990,7 +5002,7 @@
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -5001,7 +5013,7 @@
         <v>132</v>
       </c>
       <c r="C133" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -5012,7 +5024,7 @@
         <v>133</v>
       </c>
       <c r="C134" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -5023,7 +5035,7 @@
         <v>134</v>
       </c>
       <c r="C135" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -5034,7 +5046,7 @@
         <v>135</v>
       </c>
       <c r="C136" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -5045,7 +5057,7 @@
         <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -5056,7 +5068,7 @@
         <v>137</v>
       </c>
       <c r="C138" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -5067,7 +5079,7 @@
         <v>138</v>
       </c>
       <c r="C139" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -5078,7 +5090,7 @@
         <v>139</v>
       </c>
       <c r="C140" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -5089,7 +5101,7 @@
         <v>140</v>
       </c>
       <c r="C141" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -5111,7 +5123,7 @@
         <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -5122,7 +5134,7 @@
         <v>143</v>
       </c>
       <c r="C144" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -5133,7 +5145,7 @@
         <v>144</v>
       </c>
       <c r="C145" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -5144,7 +5156,7 @@
         <v>145</v>
       </c>
       <c r="C146" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -5155,7 +5167,7 @@
         <v>146</v>
       </c>
       <c r="C147" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5166,7 +5178,7 @@
         <v>147</v>
       </c>
       <c r="C148" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -5177,7 +5189,7 @@
         <v>148</v>
       </c>
       <c r="C149" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -5188,7 +5200,7 @@
         <v>149</v>
       </c>
       <c r="C150" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -5199,7 +5211,7 @@
         <v>150</v>
       </c>
       <c r="C151" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -5210,7 +5222,7 @@
         <v>151</v>
       </c>
       <c r="C152" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -5221,7 +5233,7 @@
         <v>152</v>
       </c>
       <c r="C153" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -5232,7 +5244,7 @@
         <v>153</v>
       </c>
       <c r="C154" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -5243,7 +5255,7 @@
         <v>154</v>
       </c>
       <c r="C155" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -5254,7 +5266,7 @@
         <v>155</v>
       </c>
       <c r="C156" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -5265,7 +5277,7 @@
         <v>156</v>
       </c>
       <c r="C157" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -5276,7 +5288,7 @@
         <v>157</v>
       </c>
       <c r="C158" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -5287,7 +5299,7 @@
         <v>158</v>
       </c>
       <c r="C159" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -5298,7 +5310,7 @@
         <v>159</v>
       </c>
       <c r="C160" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -5309,7 +5321,7 @@
         <v>160</v>
       </c>
       <c r="C161" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -5320,7 +5332,7 @@
         <v>161</v>
       </c>
       <c r="C162" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -5331,7 +5343,7 @@
         <v>162</v>
       </c>
       <c r="C163" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -5342,7 +5354,7 @@
         <v>163</v>
       </c>
       <c r="C164" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -5353,7 +5365,7 @@
         <v>164</v>
       </c>
       <c r="C165" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -5364,7 +5376,7 @@
         <v>165</v>
       </c>
       <c r="C166" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -5375,7 +5387,7 @@
         <v>166</v>
       </c>
       <c r="C167" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -5386,7 +5398,7 @@
         <v>167</v>
       </c>
       <c r="C168" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -5397,7 +5409,7 @@
         <v>168</v>
       </c>
       <c r="C169" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -5408,7 +5420,7 @@
         <v>169</v>
       </c>
       <c r="C170" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -5419,7 +5431,7 @@
         <v>170</v>
       </c>
       <c r="C171" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -5430,7 +5442,7 @@
         <v>171</v>
       </c>
       <c r="C172" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -5441,7 +5453,7 @@
         <v>172</v>
       </c>
       <c r="C173" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -5452,7 +5464,7 @@
         <v>173</v>
       </c>
       <c r="C174" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -5463,7 +5475,7 @@
         <v>174</v>
       </c>
       <c r="C175" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -5474,7 +5486,7 @@
         <v>175</v>
       </c>
       <c r="C176" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -5485,7 +5497,7 @@
         <v>176</v>
       </c>
       <c r="C177" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -5496,7 +5508,7 @@
         <v>177</v>
       </c>
       <c r="C178" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -5507,7 +5519,7 @@
         <v>178</v>
       </c>
       <c r="C179" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -5518,7 +5530,7 @@
         <v>179</v>
       </c>
       <c r="C180" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -5529,7 +5541,7 @@
         <v>180</v>
       </c>
       <c r="C181" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -5540,7 +5552,7 @@
         <v>181</v>
       </c>
       <c r="C182" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -5551,7 +5563,7 @@
         <v>182</v>
       </c>
       <c r="C183" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -5562,7 +5574,7 @@
         <v>183</v>
       </c>
       <c r="C184" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -5573,7 +5585,7 @@
         <v>184</v>
       </c>
       <c r="C185" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -5584,7 +5596,7 @@
         <v>185</v>
       </c>
       <c r="C186" t="s">
-        <v>1003</v>
+        <v>999</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -5595,7 +5607,7 @@
         <v>186</v>
       </c>
       <c r="C187" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
@@ -5617,7 +5629,7 @@
         <v>188</v>
       </c>
       <c r="C189" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -5628,7 +5640,7 @@
         <v>189</v>
       </c>
       <c r="C190" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
@@ -5639,7 +5651,7 @@
         <v>190</v>
       </c>
       <c r="C191" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -5650,7 +5662,7 @@
         <v>191</v>
       </c>
       <c r="C192" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -5661,7 +5673,7 @@
         <v>192</v>
       </c>
       <c r="C193" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -5672,7 +5684,7 @@
         <v>193</v>
       </c>
       <c r="C194" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -5694,7 +5706,7 @@
         <v>195</v>
       </c>
       <c r="C196" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -5705,7 +5717,7 @@
         <v>196</v>
       </c>
       <c r="C197" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -5716,7 +5728,7 @@
         <v>197</v>
       </c>
       <c r="C198" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -5727,7 +5739,7 @@
         <v>198</v>
       </c>
       <c r="C199" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -5738,7 +5750,7 @@
         <v>199</v>
       </c>
       <c r="C200" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -5760,7 +5772,7 @@
         <v>201</v>
       </c>
       <c r="C202" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -5771,7 +5783,7 @@
         <v>202</v>
       </c>
       <c r="C203" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -5782,7 +5794,7 @@
         <v>203</v>
       </c>
       <c r="C204" t="s">
-        <v>1004</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -5793,7 +5805,7 @@
         <v>204</v>
       </c>
       <c r="C205" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -5804,7 +5816,7 @@
         <v>205</v>
       </c>
       <c r="C206" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -5815,7 +5827,7 @@
         <v>206</v>
       </c>
       <c r="C207" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -5826,7 +5838,7 @@
         <v>207</v>
       </c>
       <c r="C208" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -5837,7 +5849,7 @@
         <v>208</v>
       </c>
       <c r="C209" t="s">
-        <v>1005</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -5848,7 +5860,7 @@
         <v>209</v>
       </c>
       <c r="C210" t="s">
-        <v>1006</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -5859,7 +5871,7 @@
         <v>210</v>
       </c>
       <c r="C211" t="s">
-        <v>1007</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -5870,7 +5882,7 @@
         <v>211</v>
       </c>
       <c r="C212" t="s">
-        <v>1008</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -5881,7 +5893,7 @@
         <v>212</v>
       </c>
       <c r="C213" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -5892,7 +5904,7 @@
         <v>213</v>
       </c>
       <c r="C214" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -5903,7 +5915,7 @@
         <v>214</v>
       </c>
       <c r="C215" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -5914,7 +5926,7 @@
         <v>215</v>
       </c>
       <c r="C216" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -5925,7 +5937,7 @@
         <v>216</v>
       </c>
       <c r="C217" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -5936,7 +5948,7 @@
         <v>217</v>
       </c>
       <c r="C218" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -5947,7 +5959,7 @@
         <v>218</v>
       </c>
       <c r="C219" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -5958,7 +5970,7 @@
         <v>219</v>
       </c>
       <c r="C220" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -5980,7 +5992,7 @@
         <v>221</v>
       </c>
       <c r="C222" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -5991,7 +6003,7 @@
         <v>222</v>
       </c>
       <c r="C223" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -6002,7 +6014,7 @@
         <v>223</v>
       </c>
       <c r="C224" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -6013,7 +6025,7 @@
         <v>224</v>
       </c>
       <c r="C225" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -6024,7 +6036,7 @@
         <v>225</v>
       </c>
       <c r="C226" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -6035,7 +6047,7 @@
         <v>226</v>
       </c>
       <c r="C227" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -6046,7 +6058,7 @@
         <v>227</v>
       </c>
       <c r="C228" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -6057,7 +6069,7 @@
         <v>228</v>
       </c>
       <c r="C229" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -6068,7 +6080,7 @@
         <v>229</v>
       </c>
       <c r="C230" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -6079,7 +6091,7 @@
         <v>230</v>
       </c>
       <c r="C231" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -6090,7 +6102,7 @@
         <v>231</v>
       </c>
       <c r="C232" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -6101,7 +6113,7 @@
         <v>232</v>
       </c>
       <c r="C233" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -6112,7 +6124,7 @@
         <v>233</v>
       </c>
       <c r="C234" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -6123,7 +6135,7 @@
         <v>234</v>
       </c>
       <c r="C235" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -6134,7 +6146,7 @@
         <v>235</v>
       </c>
       <c r="C236" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -6145,7 +6157,7 @@
         <v>236</v>
       </c>
       <c r="C237" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -6156,7 +6168,7 @@
         <v>237</v>
       </c>
       <c r="C238" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -6167,7 +6179,7 @@
         <v>238</v>
       </c>
       <c r="C239" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -6178,7 +6190,7 @@
         <v>239</v>
       </c>
       <c r="C240" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -6189,7 +6201,7 @@
         <v>240</v>
       </c>
       <c r="C241" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
@@ -6211,7 +6223,7 @@
         <v>242</v>
       </c>
       <c r="C243" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -6222,7 +6234,7 @@
         <v>243</v>
       </c>
       <c r="C244" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -6233,7 +6245,7 @@
         <v>244</v>
       </c>
       <c r="C245" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -6244,7 +6256,7 @@
         <v>245</v>
       </c>
       <c r="C246" t="s">
-        <v>1012</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -6255,7 +6267,7 @@
         <v>246</v>
       </c>
       <c r="C247" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
@@ -6266,7 +6278,7 @@
         <v>247</v>
       </c>
       <c r="C248" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
@@ -6277,7 +6289,7 @@
         <v>248</v>
       </c>
       <c r="C249" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
@@ -6288,7 +6300,7 @@
         <v>249</v>
       </c>
       <c r="C250" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
@@ -6299,7 +6311,7 @@
         <v>250</v>
       </c>
       <c r="C251" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -6321,7 +6333,7 @@
         <v>253</v>
       </c>
       <c r="C253" t="s">
-        <v>1013</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -6332,7 +6344,7 @@
         <v>254</v>
       </c>
       <c r="C254" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -6343,7 +6355,7 @@
         <v>255</v>
       </c>
       <c r="C255" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -6354,7 +6366,7 @@
         <v>256</v>
       </c>
       <c r="C256" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -6365,7 +6377,7 @@
         <v>257</v>
       </c>
       <c r="C257" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -6376,7 +6388,7 @@
         <v>258</v>
       </c>
       <c r="C258" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -6387,7 +6399,7 @@
         <v>259</v>
       </c>
       <c r="C259" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -6398,7 +6410,7 @@
         <v>260</v>
       </c>
       <c r="C260" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -6409,7 +6421,7 @@
         <v>261</v>
       </c>
       <c r="C261" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -6420,7 +6432,7 @@
         <v>262</v>
       </c>
       <c r="C262" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -6431,7 +6443,7 @@
         <v>263</v>
       </c>
       <c r="C263" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -6442,7 +6454,7 @@
         <v>264</v>
       </c>
       <c r="C264" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -6453,7 +6465,7 @@
         <v>265</v>
       </c>
       <c r="C265" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -6464,7 +6476,7 @@
         <v>266</v>
       </c>
       <c r="C266" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -6475,7 +6487,7 @@
         <v>267</v>
       </c>
       <c r="C267" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -6486,7 +6498,7 @@
         <v>268</v>
       </c>
       <c r="C268" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -6497,7 +6509,7 @@
         <v>269</v>
       </c>
       <c r="C269" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -6508,7 +6520,7 @@
         <v>270</v>
       </c>
       <c r="C270" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -6519,7 +6531,7 @@
         <v>271</v>
       </c>
       <c r="C271" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -6530,7 +6542,7 @@
         <v>272</v>
       </c>
       <c r="C272" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -6541,7 +6553,7 @@
         <v>273</v>
       </c>
       <c r="C273" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -6552,7 +6564,7 @@
         <v>274</v>
       </c>
       <c r="C274" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -6563,7 +6575,7 @@
         <v>275</v>
       </c>
       <c r="C275" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -6574,7 +6586,7 @@
         <v>276</v>
       </c>
       <c r="C276" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -6585,7 +6597,7 @@
         <v>277</v>
       </c>
       <c r="C277" t="s">
-        <v>1016</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -6596,7 +6608,7 @@
         <v>278</v>
       </c>
       <c r="C278" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -6607,7 +6619,7 @@
         <v>279</v>
       </c>
       <c r="C279" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -6618,7 +6630,7 @@
         <v>280</v>
       </c>
       <c r="C280" t="s">
-        <v>1017</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -6629,7 +6641,7 @@
         <v>281</v>
       </c>
       <c r="C281" t="s">
-        <v>1018</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -6640,7 +6652,7 @@
         <v>282</v>
       </c>
       <c r="C282" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -6651,7 +6663,7 @@
         <v>283</v>
       </c>
       <c r="C283" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -6662,7 +6674,7 @@
         <v>284</v>
       </c>
       <c r="C284" t="s">
-        <v>1019</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -6673,7 +6685,7 @@
         <v>285</v>
       </c>
       <c r="C285" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -6684,7 +6696,7 @@
         <v>286</v>
       </c>
       <c r="C286" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -6695,7 +6707,7 @@
         <v>287</v>
       </c>
       <c r="C287" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -6706,7 +6718,7 @@
         <v>288</v>
       </c>
       <c r="C288" t="s">
-        <v>1020</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -6717,7 +6729,7 @@
         <v>289</v>
       </c>
       <c r="C289" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -6728,7 +6740,7 @@
         <v>290</v>
       </c>
       <c r="C290" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
@@ -6739,7 +6751,7 @@
         <v>291</v>
       </c>
       <c r="C291" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
@@ -6750,7 +6762,7 @@
         <v>292</v>
       </c>
       <c r="C292" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -6761,7 +6773,7 @@
         <v>293</v>
       </c>
       <c r="C293" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
@@ -6772,7 +6784,7 @@
         <v>294</v>
       </c>
       <c r="C294" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -6783,7 +6795,7 @@
         <v>295</v>
       </c>
       <c r="C295" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -6794,7 +6806,7 @@
         <v>296</v>
       </c>
       <c r="C296" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -6805,7 +6817,7 @@
         <v>297</v>
       </c>
       <c r="C297" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -6816,7 +6828,7 @@
         <v>298</v>
       </c>
       <c r="C298" t="s">
-        <v>1021</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -6827,7 +6839,7 @@
         <v>299</v>
       </c>
       <c r="C299" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -6838,7 +6850,7 @@
         <v>300</v>
       </c>
       <c r="C300" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -6849,7 +6861,7 @@
         <v>301</v>
       </c>
       <c r="C301" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -6860,7 +6872,7 @@
         <v>302</v>
       </c>
       <c r="C302" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -6871,7 +6883,7 @@
         <v>303</v>
       </c>
       <c r="C303" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -6882,7 +6894,7 @@
         <v>304</v>
       </c>
       <c r="C304" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
@@ -6893,7 +6905,7 @@
         <v>305</v>
       </c>
       <c r="C305" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
@@ -6904,7 +6916,7 @@
         <v>306</v>
       </c>
       <c r="C306" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -6915,7 +6927,7 @@
         <v>307</v>
       </c>
       <c r="C307" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
@@ -6926,7 +6938,7 @@
         <v>308</v>
       </c>
       <c r="C308" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -6937,7 +6949,7 @@
         <v>309</v>
       </c>
       <c r="C309" t="s">
-        <v>1023</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -6948,7 +6960,7 @@
         <v>310</v>
       </c>
       <c r="C310" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -6959,7 +6971,7 @@
         <v>311</v>
       </c>
       <c r="C311" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -6970,7 +6982,7 @@
         <v>312</v>
       </c>
       <c r="C312" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -6981,7 +6993,7 @@
         <v>313</v>
       </c>
       <c r="C313" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -6992,7 +7004,7 @@
         <v>314</v>
       </c>
       <c r="C314" t="s">
-        <v>1024</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -7003,7 +7015,7 @@
         <v>315</v>
       </c>
       <c r="C315" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -7014,7 +7026,7 @@
         <v>316</v>
       </c>
       <c r="C316" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -7025,7 +7037,7 @@
         <v>317</v>
       </c>
       <c r="C317" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -7036,7 +7048,7 @@
         <v>318</v>
       </c>
       <c r="C318" t="s">
-        <v>1025</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -7047,7 +7059,7 @@
         <v>319</v>
       </c>
       <c r="C319" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -7058,7 +7070,7 @@
         <v>320</v>
       </c>
       <c r="C320" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -7069,7 +7081,7 @@
         <v>321</v>
       </c>
       <c r="C321" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -7080,7 +7092,7 @@
         <v>322</v>
       </c>
       <c r="C322" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -7091,7 +7103,7 @@
         <v>323</v>
       </c>
       <c r="C323" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -7113,7 +7125,7 @@
         <v>325</v>
       </c>
       <c r="C325" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -7124,7 +7136,7 @@
         <v>326</v>
       </c>
       <c r="C326" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -7135,7 +7147,7 @@
         <v>327</v>
       </c>
       <c r="C327" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -7146,7 +7158,7 @@
         <v>328</v>
       </c>
       <c r="C328" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -7157,7 +7169,7 @@
         <v>329</v>
       </c>
       <c r="C329" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -7168,7 +7180,7 @@
         <v>330</v>
       </c>
       <c r="C330" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -7179,7 +7191,7 @@
         <v>331</v>
       </c>
       <c r="C331" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
@@ -7201,7 +7213,7 @@
         <v>333</v>
       </c>
       <c r="C333" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
@@ -7212,7 +7224,7 @@
         <v>334</v>
       </c>
       <c r="C334" t="s">
-        <v>1026</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -7223,7 +7235,7 @@
         <v>335</v>
       </c>
       <c r="C335" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -7234,7 +7246,7 @@
         <v>336</v>
       </c>
       <c r="C336" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -7245,7 +7257,7 @@
         <v>337</v>
       </c>
       <c r="C337" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -7256,7 +7268,7 @@
         <v>338</v>
       </c>
       <c r="C338" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
@@ -7267,7 +7279,7 @@
         <v>339</v>
       </c>
       <c r="C339" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -7278,7 +7290,7 @@
         <v>340</v>
       </c>
       <c r="C340" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
@@ -7289,7 +7301,7 @@
         <v>341</v>
       </c>
       <c r="C341" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -7300,7 +7312,7 @@
         <v>342</v>
       </c>
       <c r="C342" t="s">
-        <v>1027</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -7322,7 +7334,7 @@
         <v>344</v>
       </c>
       <c r="C344" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -7333,7 +7345,7 @@
         <v>345</v>
       </c>
       <c r="C345" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -7344,7 +7356,7 @@
         <v>346</v>
       </c>
       <c r="C346" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -7355,7 +7367,7 @@
         <v>347</v>
       </c>
       <c r="C347" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -7366,7 +7378,7 @@
         <v>348</v>
       </c>
       <c r="C348" t="s">
-        <v>1028</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -7377,7 +7389,7 @@
         <v>349</v>
       </c>
       <c r="C349" t="s">
-        <v>1029</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -7388,7 +7400,7 @@
         <v>350</v>
       </c>
       <c r="C350" t="s">
-        <v>1030</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
@@ -7399,7 +7411,7 @@
         <v>351</v>
       </c>
       <c r="C351" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -7410,7 +7422,7 @@
         <v>352</v>
       </c>
       <c r="C352" t="s">
-        <v>1031</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -7421,7 +7433,7 @@
         <v>353</v>
       </c>
       <c r="C353" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -7432,7 +7444,7 @@
         <v>354</v>
       </c>
       <c r="C354" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -7454,7 +7466,7 @@
         <v>356</v>
       </c>
       <c r="C356" t="s">
-        <v>1032</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -7465,7 +7477,7 @@
         <v>357</v>
       </c>
       <c r="C357" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
@@ -7476,7 +7488,7 @@
         <v>358</v>
       </c>
       <c r="C358" t="s">
-        <v>1033</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -7487,7 +7499,7 @@
         <v>359</v>
       </c>
       <c r="C359" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -7498,7 +7510,7 @@
         <v>360</v>
       </c>
       <c r="C360" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
@@ -7509,7 +7521,7 @@
         <v>361</v>
       </c>
       <c r="C361" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
@@ -7520,7 +7532,7 @@
         <v>362</v>
       </c>
       <c r="C362" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
@@ -7531,7 +7543,7 @@
         <v>363</v>
       </c>
       <c r="C363" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -7542,7 +7554,7 @@
         <v>364</v>
       </c>
       <c r="C364" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
@@ -7553,7 +7565,7 @@
         <v>365</v>
       </c>
       <c r="C365" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -7564,7 +7576,7 @@
         <v>366</v>
       </c>
       <c r="C366" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
@@ -7575,7 +7587,7 @@
         <v>367</v>
       </c>
       <c r="C367" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
@@ -7586,7 +7598,7 @@
         <v>368</v>
       </c>
       <c r="C368" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -7597,7 +7609,7 @@
         <v>369</v>
       </c>
       <c r="C369" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -7608,7 +7620,7 @@
         <v>370</v>
       </c>
       <c r="C370" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -7619,7 +7631,7 @@
         <v>371</v>
       </c>
       <c r="C371" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -7630,7 +7642,7 @@
         <v>372</v>
       </c>
       <c r="C372" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -7652,7 +7664,7 @@
         <v>375</v>
       </c>
       <c r="C374" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -7663,7 +7675,7 @@
         <v>376</v>
       </c>
       <c r="C375" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -7674,7 +7686,7 @@
         <v>377</v>
       </c>
       <c r="C376" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
@@ -7685,7 +7697,7 @@
         <v>378</v>
       </c>
       <c r="C377" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -7696,7 +7708,7 @@
         <v>379</v>
       </c>
       <c r="C378" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -7707,7 +7719,7 @@
         <v>380</v>
       </c>
       <c r="C379" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -7718,7 +7730,7 @@
         <v>381</v>
       </c>
       <c r="C380" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -7740,7 +7752,7 @@
         <v>383</v>
       </c>
       <c r="C382" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -7751,7 +7763,7 @@
         <v>384</v>
       </c>
       <c r="C383" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -7762,7 +7774,7 @@
         <v>385</v>
       </c>
       <c r="C384" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -7773,7 +7785,7 @@
         <v>386</v>
       </c>
       <c r="C385" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -7784,7 +7796,7 @@
         <v>387</v>
       </c>
       <c r="C386" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -7795,7 +7807,7 @@
         <v>388</v>
       </c>
       <c r="C387" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -7806,7 +7818,7 @@
         <v>389</v>
       </c>
       <c r="C388" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -7817,7 +7829,7 @@
         <v>390</v>
       </c>
       <c r="C389" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
@@ -7828,7 +7840,7 @@
         <v>391</v>
       </c>
       <c r="C390" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
@@ -7839,7 +7851,7 @@
         <v>392</v>
       </c>
       <c r="C391" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
@@ -7850,7 +7862,7 @@
         <v>393</v>
       </c>
       <c r="C392" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
@@ -7872,7 +7884,7 @@
         <v>395</v>
       </c>
       <c r="C394" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -7883,7 +7895,7 @@
         <v>396</v>
       </c>
       <c r="C395" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -7894,7 +7906,7 @@
         <v>397</v>
       </c>
       <c r="C396" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -7905,7 +7917,7 @@
         <v>398</v>
       </c>
       <c r="C397" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -7916,7 +7928,7 @@
         <v>399</v>
       </c>
       <c r="C398" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -7927,7 +7939,7 @@
         <v>400</v>
       </c>
       <c r="C399" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -7938,7 +7950,7 @@
         <v>401</v>
       </c>
       <c r="C400" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
@@ -7949,7 +7961,7 @@
         <v>402</v>
       </c>
       <c r="C401" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
@@ -7960,7 +7972,7 @@
         <v>403</v>
       </c>
       <c r="C402" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
@@ -7971,7 +7983,7 @@
         <v>404</v>
       </c>
       <c r="C403" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
@@ -7982,7 +7994,7 @@
         <v>405</v>
       </c>
       <c r="C404" t="s">
-        <v>1040</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
@@ -7993,7 +8005,7 @@
         <v>406</v>
       </c>
       <c r="C405" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
@@ -8004,7 +8016,7 @@
         <v>407</v>
       </c>
       <c r="C406" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
@@ -8015,7 +8027,7 @@
         <v>408</v>
       </c>
       <c r="C407" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
@@ -8026,7 +8038,7 @@
         <v>409</v>
       </c>
       <c r="C408" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
@@ -8037,7 +8049,7 @@
         <v>410</v>
       </c>
       <c r="C409" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
@@ -8048,7 +8060,7 @@
         <v>411</v>
       </c>
       <c r="C410" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
@@ -8059,7 +8071,7 @@
         <v>412</v>
       </c>
       <c r="C411" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
@@ -8070,7 +8082,7 @@
         <v>413</v>
       </c>
       <c r="C412" t="s">
-        <v>1041</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
@@ -8081,7 +8093,7 @@
         <v>414</v>
       </c>
       <c r="C413" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
@@ -8092,7 +8104,7 @@
         <v>415</v>
       </c>
       <c r="C414" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
@@ -8103,7 +8115,7 @@
         <v>416</v>
       </c>
       <c r="C415" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
@@ -8114,7 +8126,7 @@
         <v>417</v>
       </c>
       <c r="C416" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
@@ -8125,7 +8137,7 @@
         <v>418</v>
       </c>
       <c r="C417" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
@@ -8136,7 +8148,7 @@
         <v>419</v>
       </c>
       <c r="C418" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
@@ -8147,7 +8159,7 @@
         <v>420</v>
       </c>
       <c r="C419" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
@@ -8158,7 +8170,7 @@
         <v>421</v>
       </c>
       <c r="C420" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
@@ -8169,7 +8181,7 @@
         <v>422</v>
       </c>
       <c r="C421" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
@@ -8180,7 +8192,7 @@
         <v>423</v>
       </c>
       <c r="C422" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
@@ -8191,7 +8203,7 @@
         <v>424</v>
       </c>
       <c r="C423" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
@@ -8202,7 +8214,7 @@
         <v>425</v>
       </c>
       <c r="C424" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -8213,7 +8225,7 @@
         <v>426</v>
       </c>
       <c r="C425" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
@@ -8224,7 +8236,7 @@
         <v>427</v>
       </c>
       <c r="C426" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -8235,7 +8247,7 @@
         <v>428</v>
       </c>
       <c r="C427" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
@@ -8246,7 +8258,7 @@
         <v>429</v>
       </c>
       <c r="C428" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
@@ -8257,7 +8269,7 @@
         <v>430</v>
       </c>
       <c r="C429" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
@@ -8268,7 +8280,7 @@
         <v>431</v>
       </c>
       <c r="C430" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -8279,7 +8291,7 @@
         <v>432</v>
       </c>
       <c r="C431" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -8290,7 +8302,7 @@
         <v>433</v>
       </c>
       <c r="C432" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -8301,7 +8313,7 @@
         <v>434</v>
       </c>
       <c r="C433" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -8323,7 +8335,7 @@
         <v>436</v>
       </c>
       <c r="C435" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
@@ -8334,7 +8346,7 @@
         <v>437</v>
       </c>
       <c r="C436" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
@@ -8345,7 +8357,7 @@
         <v>438</v>
       </c>
       <c r="C437" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
@@ -8356,7 +8368,7 @@
         <v>439</v>
       </c>
       <c r="C438" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
@@ -8367,7 +8379,7 @@
         <v>440</v>
       </c>
       <c r="C439" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
@@ -8378,7 +8390,7 @@
         <v>441</v>
       </c>
       <c r="C440" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.25">
@@ -8389,7 +8401,7 @@
         <v>442</v>
       </c>
       <c r="C441" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
@@ -8400,7 +8412,7 @@
         <v>443</v>
       </c>
       <c r="C442" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
@@ -8411,7 +8423,7 @@
         <v>444</v>
       </c>
       <c r="C443" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
@@ -8422,7 +8434,7 @@
         <v>445</v>
       </c>
       <c r="C444" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
@@ -8433,7 +8445,7 @@
         <v>446</v>
       </c>
       <c r="C445" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
@@ -8444,7 +8456,7 @@
         <v>447</v>
       </c>
       <c r="C446" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
@@ -8455,7 +8467,7 @@
         <v>448</v>
       </c>
       <c r="C447" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -8477,7 +8489,7 @@
         <v>450</v>
       </c>
       <c r="C449" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
@@ -8488,7 +8500,7 @@
         <v>451</v>
       </c>
       <c r="C450" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
@@ -8499,7 +8511,7 @@
         <v>452</v>
       </c>
       <c r="C451" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
@@ -8510,7 +8522,7 @@
         <v>453</v>
       </c>
       <c r="C452" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
@@ -8521,7 +8533,7 @@
         <v>454</v>
       </c>
       <c r="C453" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
@@ -8543,7 +8555,7 @@
         <v>456</v>
       </c>
       <c r="C455" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
@@ -8554,7 +8566,7 @@
         <v>457</v>
       </c>
       <c r="C456" t="s">
-        <v>1045</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
@@ -8565,7 +8577,7 @@
         <v>458</v>
       </c>
       <c r="C457" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.25">
@@ -8576,7 +8588,7 @@
         <v>459</v>
       </c>
       <c r="C458" t="s">
-        <v>1046</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
@@ -8587,7 +8599,7 @@
         <v>460</v>
       </c>
       <c r="C459" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
@@ -8598,7 +8610,7 @@
         <v>461</v>
       </c>
       <c r="C460" t="s">
-        <v>1047</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -8609,7 +8621,7 @@
         <v>462</v>
       </c>
       <c r="C461" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.25">
@@ -8620,7 +8632,7 @@
         <v>463</v>
       </c>
       <c r="C462" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
@@ -8631,7 +8643,7 @@
         <v>464</v>
       </c>
       <c r="C463" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
@@ -8642,7 +8654,7 @@
         <v>465</v>
       </c>
       <c r="C464" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
@@ -8653,7 +8665,7 @@
         <v>466</v>
       </c>
       <c r="C465" t="s">
-        <v>1048</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.25">
@@ -8664,7 +8676,7 @@
         <v>467</v>
       </c>
       <c r="C466" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
@@ -8675,7 +8687,7 @@
         <v>468</v>
       </c>
       <c r="C467" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
@@ -8686,7 +8698,7 @@
         <v>469</v>
       </c>
       <c r="C468" t="s">
-        <v>1049</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
@@ -8697,7 +8709,7 @@
         <v>470</v>
       </c>
       <c r="C469" t="s">
-        <v>1050</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
@@ -8719,18 +8731,18 @@
         <v>472</v>
       </c>
       <c r="C471" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.25">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="472" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>471</v>
       </c>
       <c r="B472" t="s">
         <v>473</v>
       </c>
-      <c r="C472" t="s">
-        <v>562</v>
+      <c r="C472" s="2" t="s">
+        <v>1060</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
@@ -8741,7 +8753,7 @@
         <v>474</v>
       </c>
       <c r="C473" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
@@ -8752,7 +8764,7 @@
         <v>475</v>
       </c>
       <c r="C474" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
@@ -8763,7 +8775,7 @@
         <v>476</v>
       </c>
       <c r="C475" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
@@ -8774,7 +8786,7 @@
         <v>477</v>
       </c>
       <c r="C476" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">
@@ -8785,7 +8797,7 @@
         <v>478</v>
       </c>
       <c r="C477" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.25">
@@ -8796,7 +8808,7 @@
         <v>479</v>
       </c>
       <c r="C478" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.25">
@@ -8807,7 +8819,7 @@
         <v>480</v>
       </c>
       <c r="C479" t="s">
-        <v>1051</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
@@ -8818,7 +8830,7 @@
         <v>481</v>
       </c>
       <c r="C480" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.25">
@@ -8829,7 +8841,7 @@
         <v>482</v>
       </c>
       <c r="C481" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
@@ -8840,18 +8852,18 @@
         <v>483</v>
       </c>
       <c r="C482" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>482</v>
       </c>
       <c r="B483" t="s">
         <v>484</v>
       </c>
-      <c r="C483" t="s">
-        <v>958</v>
+      <c r="C483" s="2" t="s">
+        <v>1059</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
@@ -8862,7 +8874,7 @@
         <v>485</v>
       </c>
       <c r="C484" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
@@ -8873,7 +8885,7 @@
         <v>486</v>
       </c>
       <c r="C485" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
@@ -8884,7 +8896,7 @@
         <v>487</v>
       </c>
       <c r="C486" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
@@ -8895,7 +8907,7 @@
         <v>488</v>
       </c>
       <c r="C487" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
@@ -8906,7 +8918,7 @@
         <v>489</v>
       </c>
       <c r="C488" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
@@ -8917,7 +8929,7 @@
         <v>490</v>
       </c>
       <c r="C489" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.25">
@@ -8928,7 +8940,7 @@
         <v>491</v>
       </c>
       <c r="C490" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.25">
@@ -8939,7 +8951,7 @@
         <v>492</v>
       </c>
       <c r="C491" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.25">
@@ -8950,7 +8962,7 @@
         <v>493</v>
       </c>
       <c r="C492" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.25">
@@ -8961,7 +8973,7 @@
         <v>494</v>
       </c>
       <c r="C493" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
@@ -8972,7 +8984,7 @@
         <v>495</v>
       </c>
       <c r="C494" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
@@ -8983,7 +8995,7 @@
         <v>496</v>
       </c>
       <c r="C495" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
@@ -8994,7 +9006,7 @@
         <v>497</v>
       </c>
       <c r="C496" t="s">
-        <v>1052</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -9005,7 +9017,7 @@
         <v>498</v>
       </c>
       <c r="C497" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
@@ -9016,7 +9028,7 @@
         <v>499</v>
       </c>
       <c r="C498" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
@@ -9027,7 +9039,7 @@
         <v>500</v>
       </c>
       <c r="C499" t="s">
-        <v>1053</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.25">
@@ -9038,7 +9050,7 @@
         <v>501</v>
       </c>
       <c r="C500" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.25">
@@ -9049,7 +9061,7 @@
         <v>502</v>
       </c>
       <c r="C501" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
@@ -9060,7 +9072,7 @@
         <v>503</v>
       </c>
       <c r="C502" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.25">
@@ -9071,7 +9083,7 @@
         <v>504</v>
       </c>
       <c r="C503" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.25">
@@ -9082,7 +9094,7 @@
         <v>505</v>
       </c>
       <c r="C504" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
@@ -9093,7 +9105,7 @@
         <v>506</v>
       </c>
       <c r="C505" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="506" spans="1:3" x14ac:dyDescent="0.25">
@@ -9104,7 +9116,7 @@
         <v>507</v>
       </c>
       <c r="C506" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="507" spans="1:3" x14ac:dyDescent="0.25">
@@ -9115,7 +9127,7 @@
         <v>508</v>
       </c>
       <c r="C507" t="s">
-        <v>1054</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
@@ -9126,7 +9138,7 @@
         <v>509</v>
       </c>
       <c r="C508" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.25">
@@ -9137,7 +9149,7 @@
         <v>510</v>
       </c>
       <c r="C509" t="s">
-        <v>968</v>
+        <v>964</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
@@ -9148,7 +9160,7 @@
         <v>511</v>
       </c>
       <c r="C510" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="511" spans="1:3" x14ac:dyDescent="0.25">
@@ -9159,7 +9171,7 @@
         <v>512</v>
       </c>
       <c r="C511" t="s">
-        <v>969</v>
+        <v>965</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
@@ -9170,7 +9182,7 @@
         <v>513</v>
       </c>
       <c r="C512" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="513" spans="1:3" x14ac:dyDescent="0.25">
@@ -9181,7 +9193,7 @@
         <v>514</v>
       </c>
       <c r="C513" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="514" spans="1:3" x14ac:dyDescent="0.25">
@@ -9192,7 +9204,7 @@
         <v>515</v>
       </c>
       <c r="C514" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="515" spans="1:3" x14ac:dyDescent="0.25">
@@ -9203,7 +9215,7 @@
         <v>516</v>
       </c>
       <c r="C515" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="516" spans="1:3" x14ac:dyDescent="0.25">
@@ -9214,7 +9226,7 @@
         <v>517</v>
       </c>
       <c r="C516" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="517" spans="1:3" x14ac:dyDescent="0.25">
@@ -9225,18 +9237,18 @@
         <v>518</v>
       </c>
       <c r="C517" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="518" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A518">
         <v>517</v>
       </c>
       <c r="B518" t="s">
         <v>519</v>
       </c>
-      <c r="C518" t="s">
-        <v>931</v>
+      <c r="C518" s="2" t="s">
+        <v>1058</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
@@ -9247,7 +9259,7 @@
         <v>520</v>
       </c>
       <c r="C519" t="s">
-        <v>1055</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.25">
@@ -9258,7 +9270,7 @@
         <v>521</v>
       </c>
       <c r="C520" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
@@ -9269,7 +9281,7 @@
         <v>522</v>
       </c>
       <c r="C521" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="522" spans="1:3" x14ac:dyDescent="0.25">
@@ -9280,7 +9292,7 @@
         <v>523</v>
       </c>
       <c r="C522" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="523" spans="1:3" x14ac:dyDescent="0.25">
@@ -9291,7 +9303,7 @@
         <v>524</v>
       </c>
       <c r="C523" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="524" spans="1:3" x14ac:dyDescent="0.25">
@@ -9302,7 +9314,7 @@
         <v>525</v>
       </c>
       <c r="C524" t="s">
-        <v>970</v>
+        <v>966</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
@@ -9313,7 +9325,7 @@
         <v>535</v>
       </c>
       <c r="C525" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.25">
@@ -9324,7 +9336,7 @@
         <v>526</v>
       </c>
       <c r="C526" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.25">
@@ -9335,7 +9347,7 @@
         <v>527</v>
       </c>
       <c r="C527" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.25">
@@ -9346,7 +9358,7 @@
         <v>528</v>
       </c>
       <c r="C528" t="s">
-        <v>1057</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.25">
@@ -9357,7 +9369,7 @@
         <v>529</v>
       </c>
       <c r="C529" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="530" spans="1:3" x14ac:dyDescent="0.25">
@@ -9368,7 +9380,7 @@
         <v>530</v>
       </c>
       <c r="C530" t="s">
-        <v>971</v>
+        <v>967</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
@@ -9379,7 +9391,7 @@
         <v>531</v>
       </c>
       <c r="C531" t="s">
-        <v>972</v>
+        <v>968</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.25">
@@ -9390,7 +9402,7 @@
         <v>532</v>
       </c>
       <c r="C532" t="s">
-        <v>973</v>
+        <v>969</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.25">
@@ -9401,7 +9413,7 @@
         <v>533</v>
       </c>
       <c r="C533" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">
@@ -9412,7 +9424,7 @@
         <v>534</v>
       </c>
       <c r="C534" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing a find and replace error
</commit_message>
<xml_diff>
--- a/UnityProject/LD35/Assets/StaticDefinitions/BeetleNameDefs.xlsx
+++ b/UnityProject/LD35/Assets/StaticDefinitions/BeetleNameDefs.xlsx
@@ -2432,9 +2432,6 @@
     <t xml:space="preserve">Phalacrus politus </t>
   </si>
   <si>
-    <t>Chrysomela i</t>
-  </si>
-  <si>
     <t xml:space="preserve">Epitrix fuscula </t>
   </si>
   <si>
@@ -3214,6 +3211,9 @@
   <si>
     <t>Callidium antennatum
 hesperum</t>
+  </si>
+  <si>
+    <t>Chrysomela crotchi</t>
   </si>
 </sst>
 </file>
@@ -3543,8 +3543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C534"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3555,13 +3555,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3814,7 +3814,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>802</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -4100,7 +4100,7 @@
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -4111,7 +4111,7 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -4122,7 +4122,7 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -4155,7 +4155,7 @@
         <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4166,7 +4166,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -4177,7 +4177,7 @@
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -4397,7 +4397,7 @@
         <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -4441,7 +4441,7 @@
         <v>80</v>
       </c>
       <c r="C81" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -4463,7 +4463,7 @@
         <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -4573,7 +4573,7 @@
         <v>92</v>
       </c>
       <c r="C93" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -4606,7 +4606,7 @@
         <v>95</v>
       </c>
       <c r="C96" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -4672,7 +4672,7 @@
         <v>101</v>
       </c>
       <c r="C102" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -4683,7 +4683,7 @@
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -4749,7 +4749,7 @@
         <v>108</v>
       </c>
       <c r="C109" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -4848,7 +4848,7 @@
         <v>117</v>
       </c>
       <c r="C118" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -4870,7 +4870,7 @@
         <v>119</v>
       </c>
       <c r="C120" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -4903,7 +4903,7 @@
         <v>122</v>
       </c>
       <c r="C123" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -4914,7 +4914,7 @@
         <v>123</v>
       </c>
       <c r="C124" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -4947,7 +4947,7 @@
         <v>126</v>
       </c>
       <c r="C127" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -4958,7 +4958,7 @@
         <v>127</v>
       </c>
       <c r="C128" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -4969,7 +4969,7 @@
         <v>128</v>
       </c>
       <c r="C129" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -4980,7 +4980,7 @@
         <v>129</v>
       </c>
       <c r="C130" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
         <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -5002,7 +5002,7 @@
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -5013,7 +5013,7 @@
         <v>132</v>
       </c>
       <c r="C133" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -5035,7 +5035,7 @@
         <v>134</v>
       </c>
       <c r="C135" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -5057,7 +5057,7 @@
         <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -5101,7 +5101,7 @@
         <v>140</v>
       </c>
       <c r="C141" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -5123,7 +5123,7 @@
         <v>142</v>
       </c>
       <c r="C143" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -5145,7 +5145,7 @@
         <v>144</v>
       </c>
       <c r="C145" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -5156,7 +5156,7 @@
         <v>145</v>
       </c>
       <c r="C146" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -5167,7 +5167,7 @@
         <v>146</v>
       </c>
       <c r="C147" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -5178,7 +5178,7 @@
         <v>147</v>
       </c>
       <c r="C148" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -5211,7 +5211,7 @@
         <v>150</v>
       </c>
       <c r="C151" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -5222,7 +5222,7 @@
         <v>151</v>
       </c>
       <c r="C152" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -5255,7 +5255,7 @@
         <v>154</v>
       </c>
       <c r="C155" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -5266,7 +5266,7 @@
         <v>155</v>
       </c>
       <c r="C156" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -5288,7 +5288,7 @@
         <v>157</v>
       </c>
       <c r="C158" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
@@ -5299,7 +5299,7 @@
         <v>158</v>
       </c>
       <c r="C159" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -5321,7 +5321,7 @@
         <v>160</v>
       </c>
       <c r="C161" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -5332,7 +5332,7 @@
         <v>161</v>
       </c>
       <c r="C162" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -5376,7 +5376,7 @@
         <v>165</v>
       </c>
       <c r="C166" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -5398,7 +5398,7 @@
         <v>167</v>
       </c>
       <c r="C168" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -5431,7 +5431,7 @@
         <v>170</v>
       </c>
       <c r="C171" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -5442,7 +5442,7 @@
         <v>171</v>
       </c>
       <c r="C172" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -5464,7 +5464,7 @@
         <v>173</v>
       </c>
       <c r="C174" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -5475,7 +5475,7 @@
         <v>174</v>
       </c>
       <c r="C175" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -5486,7 +5486,7 @@
         <v>175</v>
       </c>
       <c r="C176" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -5519,7 +5519,7 @@
         <v>178</v>
       </c>
       <c r="C179" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -5530,7 +5530,7 @@
         <v>179</v>
       </c>
       <c r="C180" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -5541,7 +5541,7 @@
         <v>180</v>
       </c>
       <c r="C181" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -5552,7 +5552,7 @@
         <v>181</v>
       </c>
       <c r="C182" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -5563,7 +5563,7 @@
         <v>182</v>
       </c>
       <c r="C183" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
@@ -5574,7 +5574,7 @@
         <v>183</v>
       </c>
       <c r="C184" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -5585,7 +5585,7 @@
         <v>184</v>
       </c>
       <c r="C185" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -5596,7 +5596,7 @@
         <v>185</v>
       </c>
       <c r="C186" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -5629,7 +5629,7 @@
         <v>188</v>
       </c>
       <c r="C189" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
@@ -5706,7 +5706,7 @@
         <v>195</v>
       </c>
       <c r="C196" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -5717,7 +5717,7 @@
         <v>196</v>
       </c>
       <c r="C197" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -5728,7 +5728,7 @@
         <v>197</v>
       </c>
       <c r="C198" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -5750,7 +5750,7 @@
         <v>199</v>
       </c>
       <c r="C200" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -5772,7 +5772,7 @@
         <v>201</v>
       </c>
       <c r="C202" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -5794,7 +5794,7 @@
         <v>203</v>
       </c>
       <c r="C204" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -5816,7 +5816,7 @@
         <v>205</v>
       </c>
       <c r="C206" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -5849,7 +5849,7 @@
         <v>208</v>
       </c>
       <c r="C209" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -5860,7 +5860,7 @@
         <v>209</v>
       </c>
       <c r="C210" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -5871,7 +5871,7 @@
         <v>210</v>
       </c>
       <c r="C211" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
@@ -5882,7 +5882,7 @@
         <v>211</v>
       </c>
       <c r="C212" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -5893,7 +5893,7 @@
         <v>212</v>
       </c>
       <c r="C213" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -5937,7 +5937,7 @@
         <v>216</v>
       </c>
       <c r="C217" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -5948,7 +5948,7 @@
         <v>217</v>
       </c>
       <c r="C218" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -5959,7 +5959,7 @@
         <v>218</v>
       </c>
       <c r="C219" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -5970,7 +5970,7 @@
         <v>219</v>
       </c>
       <c r="C220" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -6003,7 +6003,7 @@
         <v>222</v>
       </c>
       <c r="C223" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -6014,7 +6014,7 @@
         <v>223</v>
       </c>
       <c r="C224" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -6025,7 +6025,7 @@
         <v>224</v>
       </c>
       <c r="C225" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -6058,7 +6058,7 @@
         <v>227</v>
       </c>
       <c r="C228" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -6080,7 +6080,7 @@
         <v>229</v>
       </c>
       <c r="C230" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -6091,7 +6091,7 @@
         <v>230</v>
       </c>
       <c r="C231" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -6102,7 +6102,7 @@
         <v>231</v>
       </c>
       <c r="C232" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -6113,7 +6113,7 @@
         <v>232</v>
       </c>
       <c r="C233" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -6124,7 +6124,7 @@
         <v>233</v>
       </c>
       <c r="C234" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -6135,7 +6135,7 @@
         <v>234</v>
       </c>
       <c r="C235" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -6146,7 +6146,7 @@
         <v>235</v>
       </c>
       <c r="C236" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -6157,7 +6157,7 @@
         <v>236</v>
       </c>
       <c r="C237" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -6179,7 +6179,7 @@
         <v>238</v>
       </c>
       <c r="C239" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -6190,7 +6190,7 @@
         <v>239</v>
       </c>
       <c r="C240" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -6223,7 +6223,7 @@
         <v>242</v>
       </c>
       <c r="C243" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
@@ -6234,7 +6234,7 @@
         <v>243</v>
       </c>
       <c r="C244" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -6245,7 +6245,7 @@
         <v>244</v>
       </c>
       <c r="C245" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
@@ -6256,7 +6256,7 @@
         <v>245</v>
       </c>
       <c r="C246" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
@@ -6311,7 +6311,7 @@
         <v>250</v>
       </c>
       <c r="C251" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -6333,7 +6333,7 @@
         <v>253</v>
       </c>
       <c r="C253" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -6344,7 +6344,7 @@
         <v>254</v>
       </c>
       <c r="C254" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -6355,7 +6355,7 @@
         <v>255</v>
       </c>
       <c r="C255" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -6377,7 +6377,7 @@
         <v>257</v>
       </c>
       <c r="C257" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -6399,7 +6399,7 @@
         <v>259</v>
       </c>
       <c r="C259" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -6421,7 +6421,7 @@
         <v>261</v>
       </c>
       <c r="C261" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -6432,7 +6432,7 @@
         <v>262</v>
       </c>
       <c r="C262" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -6443,7 +6443,7 @@
         <v>263</v>
       </c>
       <c r="C263" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -6454,7 +6454,7 @@
         <v>264</v>
       </c>
       <c r="C264" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -6465,7 +6465,7 @@
         <v>265</v>
       </c>
       <c r="C265" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -6487,7 +6487,7 @@
         <v>267</v>
       </c>
       <c r="C267" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -6498,7 +6498,7 @@
         <v>268</v>
       </c>
       <c r="C268" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -6520,7 +6520,7 @@
         <v>270</v>
       </c>
       <c r="C270" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -6531,7 +6531,7 @@
         <v>271</v>
       </c>
       <c r="C271" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
         <v>272</v>
       </c>
       <c r="C272" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -6553,7 +6553,7 @@
         <v>273</v>
       </c>
       <c r="C273" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -6564,7 +6564,7 @@
         <v>274</v>
       </c>
       <c r="C274" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -6575,7 +6575,7 @@
         <v>275</v>
       </c>
       <c r="C275" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -6586,7 +6586,7 @@
         <v>276</v>
       </c>
       <c r="C276" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -6597,7 +6597,7 @@
         <v>277</v>
       </c>
       <c r="C277" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -6608,7 +6608,7 @@
         <v>278</v>
       </c>
       <c r="C278" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -6619,7 +6619,7 @@
         <v>279</v>
       </c>
       <c r="C279" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -6630,7 +6630,7 @@
         <v>280</v>
       </c>
       <c r="C280" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -6641,7 +6641,7 @@
         <v>281</v>
       </c>
       <c r="C281" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -6674,7 +6674,7 @@
         <v>284</v>
       </c>
       <c r="C284" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -6696,7 +6696,7 @@
         <v>286</v>
       </c>
       <c r="C286" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -6718,7 +6718,7 @@
         <v>288</v>
       </c>
       <c r="C288" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
@@ -6729,7 +6729,7 @@
         <v>289</v>
       </c>
       <c r="C289" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -6762,7 +6762,7 @@
         <v>292</v>
       </c>
       <c r="C292" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -6784,7 +6784,7 @@
         <v>294</v>
       </c>
       <c r="C294" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
@@ -6795,7 +6795,7 @@
         <v>295</v>
       </c>
       <c r="C295" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
@@ -6806,7 +6806,7 @@
         <v>296</v>
       </c>
       <c r="C296" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
@@ -6817,7 +6817,7 @@
         <v>297</v>
       </c>
       <c r="C297" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
@@ -6828,7 +6828,7 @@
         <v>298</v>
       </c>
       <c r="C298" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
@@ -6839,7 +6839,7 @@
         <v>299</v>
       </c>
       <c r="C299" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
@@ -6850,7 +6850,7 @@
         <v>300</v>
       </c>
       <c r="C300" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -6861,7 +6861,7 @@
         <v>301</v>
       </c>
       <c r="C301" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -6883,7 +6883,7 @@
         <v>303</v>
       </c>
       <c r="C303" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
@@ -6938,7 +6938,7 @@
         <v>308</v>
       </c>
       <c r="C308" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
@@ -6949,7 +6949,7 @@
         <v>309</v>
       </c>
       <c r="C309" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
@@ -6971,7 +6971,7 @@
         <v>311</v>
       </c>
       <c r="C311" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -6993,7 +6993,7 @@
         <v>313</v>
       </c>
       <c r="C313" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -7004,7 +7004,7 @@
         <v>314</v>
       </c>
       <c r="C314" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -7048,7 +7048,7 @@
         <v>318</v>
       </c>
       <c r="C318" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -7059,7 +7059,7 @@
         <v>319</v>
       </c>
       <c r="C319" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
@@ -7070,7 +7070,7 @@
         <v>320</v>
       </c>
       <c r="C320" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -7081,7 +7081,7 @@
         <v>321</v>
       </c>
       <c r="C321" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -7092,7 +7092,7 @@
         <v>322</v>
       </c>
       <c r="C322" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -7103,7 +7103,7 @@
         <v>323</v>
       </c>
       <c r="C323" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -7125,7 +7125,7 @@
         <v>325</v>
       </c>
       <c r="C325" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -7136,7 +7136,7 @@
         <v>326</v>
       </c>
       <c r="C326" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -7158,7 +7158,7 @@
         <v>328</v>
       </c>
       <c r="C328" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -7224,7 +7224,7 @@
         <v>334</v>
       </c>
       <c r="C334" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -7246,7 +7246,7 @@
         <v>336</v>
       </c>
       <c r="C336" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
@@ -7257,7 +7257,7 @@
         <v>337</v>
       </c>
       <c r="C337" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
@@ -7279,7 +7279,7 @@
         <v>339</v>
       </c>
       <c r="C339" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
@@ -7301,7 +7301,7 @@
         <v>341</v>
       </c>
       <c r="C341" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
@@ -7312,7 +7312,7 @@
         <v>342</v>
       </c>
       <c r="C342" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
@@ -7334,7 +7334,7 @@
         <v>344</v>
       </c>
       <c r="C344" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
@@ -7345,7 +7345,7 @@
         <v>345</v>
       </c>
       <c r="C345" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
@@ -7356,7 +7356,7 @@
         <v>346</v>
       </c>
       <c r="C346" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
@@ -7367,7 +7367,7 @@
         <v>347</v>
       </c>
       <c r="C347" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
@@ -7378,7 +7378,7 @@
         <v>348</v>
       </c>
       <c r="C348" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
@@ -7389,7 +7389,7 @@
         <v>349</v>
       </c>
       <c r="C349" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
@@ -7400,7 +7400,7 @@
         <v>350</v>
       </c>
       <c r="C350" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
@@ -7411,7 +7411,7 @@
         <v>351</v>
       </c>
       <c r="C351" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -7422,7 +7422,7 @@
         <v>352</v>
       </c>
       <c r="C352" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
@@ -7433,7 +7433,7 @@
         <v>353</v>
       </c>
       <c r="C353" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
@@ -7444,7 +7444,7 @@
         <v>354</v>
       </c>
       <c r="C354" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
@@ -7466,7 +7466,7 @@
         <v>356</v>
       </c>
       <c r="C356" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
@@ -7488,7 +7488,7 @@
         <v>358</v>
       </c>
       <c r="C358" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
@@ -7499,7 +7499,7 @@
         <v>359</v>
       </c>
       <c r="C359" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
@@ -7532,7 +7532,7 @@
         <v>362</v>
       </c>
       <c r="C362" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
@@ -7543,7 +7543,7 @@
         <v>363</v>
       </c>
       <c r="C363" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
@@ -7565,7 +7565,7 @@
         <v>365</v>
       </c>
       <c r="C365" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
@@ -7598,7 +7598,7 @@
         <v>368</v>
       </c>
       <c r="C368" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -7675,7 +7675,7 @@
         <v>376</v>
       </c>
       <c r="C375" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -7697,7 +7697,7 @@
         <v>378</v>
       </c>
       <c r="C377" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -7708,7 +7708,7 @@
         <v>379</v>
       </c>
       <c r="C378" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -7752,7 +7752,7 @@
         <v>383</v>
       </c>
       <c r="C382" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -7763,7 +7763,7 @@
         <v>384</v>
       </c>
       <c r="C383" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -7774,7 +7774,7 @@
         <v>385</v>
       </c>
       <c r="C384" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -7785,7 +7785,7 @@
         <v>386</v>
       </c>
       <c r="C385" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -7796,7 +7796,7 @@
         <v>387</v>
       </c>
       <c r="C386" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -7829,7 +7829,7 @@
         <v>390</v>
       </c>
       <c r="C389" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
@@ -7840,7 +7840,7 @@
         <v>391</v>
       </c>
       <c r="C390" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
@@ -7851,7 +7851,7 @@
         <v>392</v>
       </c>
       <c r="C391" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
@@ -7862,7 +7862,7 @@
         <v>393</v>
       </c>
       <c r="C392" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
@@ -7884,7 +7884,7 @@
         <v>395</v>
       </c>
       <c r="C394" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -7928,7 +7928,7 @@
         <v>399</v>
       </c>
       <c r="C398" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -7939,7 +7939,7 @@
         <v>400</v>
       </c>
       <c r="C399" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -7950,7 +7950,7 @@
         <v>401</v>
       </c>
       <c r="C400" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
@@ -7961,7 +7961,7 @@
         <v>402</v>
       </c>
       <c r="C401" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
@@ -7972,7 +7972,7 @@
         <v>403</v>
       </c>
       <c r="C402" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
@@ -7983,7 +7983,7 @@
         <v>404</v>
       </c>
       <c r="C403" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
@@ -7994,7 +7994,7 @@
         <v>405</v>
       </c>
       <c r="C404" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
@@ -8005,7 +8005,7 @@
         <v>406</v>
       </c>
       <c r="C405" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
@@ -8016,7 +8016,7 @@
         <v>407</v>
       </c>
       <c r="C406" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
@@ -8027,7 +8027,7 @@
         <v>408</v>
       </c>
       <c r="C407" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
@@ -8082,7 +8082,7 @@
         <v>413</v>
       </c>
       <c r="C412" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
@@ -8093,7 +8093,7 @@
         <v>414</v>
       </c>
       <c r="C413" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
@@ -8104,7 +8104,7 @@
         <v>415</v>
       </c>
       <c r="C414" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
@@ -8126,7 +8126,7 @@
         <v>417</v>
       </c>
       <c r="C416" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
@@ -8159,7 +8159,7 @@
         <v>420</v>
       </c>
       <c r="C419" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
@@ -8170,7 +8170,7 @@
         <v>421</v>
       </c>
       <c r="C420" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
@@ -8192,7 +8192,7 @@
         <v>423</v>
       </c>
       <c r="C422" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
@@ -8203,7 +8203,7 @@
         <v>424</v>
       </c>
       <c r="C423" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
@@ -8214,7 +8214,7 @@
         <v>425</v>
       </c>
       <c r="C424" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -8236,7 +8236,7 @@
         <v>427</v>
       </c>
       <c r="C426" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -8247,7 +8247,7 @@
         <v>428</v>
       </c>
       <c r="C427" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
@@ -8258,7 +8258,7 @@
         <v>429</v>
       </c>
       <c r="C428" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
@@ -8269,7 +8269,7 @@
         <v>430</v>
       </c>
       <c r="C429" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
@@ -8291,7 +8291,7 @@
         <v>432</v>
       </c>
       <c r="C431" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -8302,7 +8302,7 @@
         <v>433</v>
       </c>
       <c r="C432" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -8335,7 +8335,7 @@
         <v>436</v>
       </c>
       <c r="C435" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
@@ -8346,7 +8346,7 @@
         <v>437</v>
       </c>
       <c r="C436" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
@@ -8368,7 +8368,7 @@
         <v>439</v>
       </c>
       <c r="C438" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
@@ -8379,7 +8379,7 @@
         <v>440</v>
       </c>
       <c r="C439" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
@@ -8412,7 +8412,7 @@
         <v>443</v>
       </c>
       <c r="C442" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
@@ -8423,7 +8423,7 @@
         <v>444</v>
       </c>
       <c r="C443" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
@@ -8434,7 +8434,7 @@
         <v>445</v>
       </c>
       <c r="C444" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
@@ -8445,7 +8445,7 @@
         <v>446</v>
       </c>
       <c r="C445" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
@@ -8467,7 +8467,7 @@
         <v>448</v>
       </c>
       <c r="C447" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -8489,7 +8489,7 @@
         <v>450</v>
       </c>
       <c r="C449" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
@@ -8533,7 +8533,7 @@
         <v>454</v>
       </c>
       <c r="C453" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
@@ -8566,7 +8566,7 @@
         <v>457</v>
       </c>
       <c r="C456" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
@@ -8588,7 +8588,7 @@
         <v>459</v>
       </c>
       <c r="C458" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
@@ -8610,7 +8610,7 @@
         <v>461</v>
       </c>
       <c r="C460" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -8654,7 +8654,7 @@
         <v>465</v>
       </c>
       <c r="C464" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
@@ -8665,7 +8665,7 @@
         <v>466</v>
       </c>
       <c r="C465" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.25">
@@ -8676,7 +8676,7 @@
         <v>467</v>
       </c>
       <c r="C466" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
@@ -8687,7 +8687,7 @@
         <v>468</v>
       </c>
       <c r="C467" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
@@ -8698,7 +8698,7 @@
         <v>469</v>
       </c>
       <c r="C468" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
@@ -8709,7 +8709,7 @@
         <v>470</v>
       </c>
       <c r="C469" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
@@ -8731,7 +8731,7 @@
         <v>472</v>
       </c>
       <c r="C471" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="472" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -8742,7 +8742,7 @@
         <v>473</v>
       </c>
       <c r="C472" s="2" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
@@ -8753,7 +8753,7 @@
         <v>474</v>
       </c>
       <c r="C473" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
@@ -8797,7 +8797,7 @@
         <v>478</v>
       </c>
       <c r="C477" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.25">
@@ -8819,7 +8819,7 @@
         <v>480</v>
       </c>
       <c r="C479" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
@@ -8852,7 +8852,7 @@
         <v>483</v>
       </c>
       <c r="C482" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="483" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -8863,7 +8863,7 @@
         <v>484</v>
       </c>
       <c r="C483" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
@@ -8874,7 +8874,7 @@
         <v>485</v>
       </c>
       <c r="C484" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
@@ -8885,7 +8885,7 @@
         <v>486</v>
       </c>
       <c r="C485" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
@@ -8896,7 +8896,7 @@
         <v>487</v>
       </c>
       <c r="C486" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
@@ -8907,7 +8907,7 @@
         <v>488</v>
       </c>
       <c r="C487" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
@@ -8973,7 +8973,7 @@
         <v>494</v>
       </c>
       <c r="C493" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
@@ -9006,7 +9006,7 @@
         <v>497</v>
       </c>
       <c r="C496" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -9017,7 +9017,7 @@
         <v>498</v>
       </c>
       <c r="C497" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
@@ -9039,7 +9039,7 @@
         <v>500</v>
       </c>
       <c r="C499" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.25">
@@ -9050,7 +9050,7 @@
         <v>501</v>
       </c>
       <c r="C500" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.25">
@@ -9061,7 +9061,7 @@
         <v>502</v>
       </c>
       <c r="C501" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
@@ -9072,7 +9072,7 @@
         <v>503</v>
       </c>
       <c r="C502" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="503" spans="1:3" x14ac:dyDescent="0.25">
@@ -9083,7 +9083,7 @@
         <v>504</v>
       </c>
       <c r="C503" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="504" spans="1:3" x14ac:dyDescent="0.25">
@@ -9094,7 +9094,7 @@
         <v>505</v>
       </c>
       <c r="C504" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="505" spans="1:3" x14ac:dyDescent="0.25">
@@ -9127,7 +9127,7 @@
         <v>508</v>
       </c>
       <c r="C507" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="508" spans="1:3" x14ac:dyDescent="0.25">
@@ -9149,7 +9149,7 @@
         <v>510</v>
       </c>
       <c r="C509" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="510" spans="1:3" x14ac:dyDescent="0.25">
@@ -9171,7 +9171,7 @@
         <v>512</v>
       </c>
       <c r="C511" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
@@ -9248,7 +9248,7 @@
         <v>519</v>
       </c>
       <c r="C518" s="2" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="519" spans="1:3" x14ac:dyDescent="0.25">
@@ -9259,7 +9259,7 @@
         <v>520</v>
       </c>
       <c r="C519" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="520" spans="1:3" x14ac:dyDescent="0.25">
@@ -9270,7 +9270,7 @@
         <v>521</v>
       </c>
       <c r="C520" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="521" spans="1:3" x14ac:dyDescent="0.25">
@@ -9314,7 +9314,7 @@
         <v>525</v>
       </c>
       <c r="C524" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="525" spans="1:3" x14ac:dyDescent="0.25">
@@ -9325,7 +9325,7 @@
         <v>535</v>
       </c>
       <c r="C525" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="526" spans="1:3" x14ac:dyDescent="0.25">
@@ -9358,7 +9358,7 @@
         <v>528</v>
       </c>
       <c r="C528" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="529" spans="1:3" x14ac:dyDescent="0.25">
@@ -9380,7 +9380,7 @@
         <v>530</v>
       </c>
       <c r="C530" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
@@ -9391,7 +9391,7 @@
         <v>531</v>
       </c>
       <c r="C531" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="532" spans="1:3" x14ac:dyDescent="0.25">
@@ -9402,7 +9402,7 @@
         <v>532</v>
       </c>
       <c r="C532" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="533" spans="1:3" x14ac:dyDescent="0.25">
@@ -9413,7 +9413,7 @@
         <v>533</v>
       </c>
       <c r="C533" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="534" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>